<commit_message>
CARLA-UPDATE LEAVE CARD 3/29/2023 4:25 PM
</commit_message>
<xml_diff>
--- a/JOBCON/CONSTANTE, HERBERT FELICIANO.xlsx
+++ b/JOBCON/CONSTANTE, HERBERT FELICIANO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\DESKTOP-44REB32\Users\ASUS\Desktop\LEAVECARD\JOBCON\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DOLE\Desktop\LEAVE-CARD\JOBCON\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
   <si>
     <t>PERIOD</t>
   </si>
@@ -195,6 +195,15 @@
   </si>
   <si>
     <t>SL(7-0-0)</t>
+  </si>
+  <si>
+    <t>3/12,16,17/2023</t>
+  </si>
+  <si>
+    <t>SL(2-0-0)</t>
+  </si>
+  <si>
+    <t>3/6,8/2023</t>
   </si>
 </sst>
 </file>
@@ -891,7 +900,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -934,7 +943,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -998,7 +1007,7 @@
         <xdr:cNvPr id="4" name="Arrow: Left 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1058,7 +1067,7 @@
         <xdr:cNvPr id="8" name="Oval 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1124,7 +1133,7 @@
         <xdr:cNvPr id="9" name="Arrow: Left-Right 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1187,7 +1196,7 @@
         <xdr:cNvPr id="10" name="TextBox 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1285,7 +1294,7 @@
         <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1344,7 +1353,7 @@
         <xdr:cNvPr id="19" name="TextBox 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1409,7 +1418,7 @@
         <xdr:cNvPr id="20" name="Picture 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1452,7 +1461,7 @@
         <xdr:cNvPr id="21" name="TextBox 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1527,7 +1536,7 @@
         <xdr:cNvPr id="22" name="TextBox 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1713,7 +1722,7 @@
         <xdr:cNvPr id="23" name="Oval 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1779,7 +1788,7 @@
         <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1837,7 +1846,7 @@
         <xdr:cNvPr id="26" name="Oval 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1903,7 +1912,7 @@
         <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1959,7 +1968,7 @@
         <xdr:cNvPr id="30" name="TextBox 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2034,7 +2043,7 @@
         <xdr:cNvPr id="31" name="Picture 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2077,7 +2086,7 @@
         <xdr:cNvPr id="32" name="Oval 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2143,7 +2152,7 @@
         <xdr:cNvPr id="33" name="Straight Arrow Connector 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2199,7 +2208,7 @@
         <xdr:cNvPr id="34" name="TextBox 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2295,7 +2304,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:K130" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:K131" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <tableColumns count="11">
     <tableColumn id="1" name="PERIOD" dataDxfId="10"/>
     <tableColumn id="2" name="PARTICULARS" dataDxfId="9"/>
@@ -2642,12 +2651,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:K130"/>
+  <dimension ref="A2:K131"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3570" topLeftCell="A10" activePane="bottomLeft"/>
       <selection activeCell="F3" sqref="F3:G3"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2921,8 +2930,12 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="42"/>
-      <c r="B14" s="21"/>
+      <c r="A14" s="42">
+        <v>37324</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>52</v>
+      </c>
       <c r="C14" s="14"/>
       <c r="D14" s="41"/>
       <c r="E14" s="10"/>
@@ -2933,12 +2946,20 @@
       </c>
       <c r="H14" s="41"/>
       <c r="I14" s="10"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="21"/>
+      <c r="J14" s="12">
+        <v>2</v>
+      </c>
+      <c r="K14" s="21" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="42"/>
-      <c r="B15" s="21"/>
+      <c r="A15" s="42">
+        <v>45005</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>46</v>
+      </c>
       <c r="C15" s="14"/>
       <c r="D15" s="41"/>
       <c r="E15" s="10"/>
@@ -2949,40 +2970,44 @@
       </c>
       <c r="H15" s="41"/>
       <c r="I15" s="10"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="21"/>
+      <c r="J15" s="12">
+        <v>3</v>
+      </c>
+      <c r="K15" s="21" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="43"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="45"/>
+      <c r="A16" s="42"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="41"/>
       <c r="E16" s="10"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="44" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H16" s="45"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="14" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H16" s="41"/>
       <c r="I16" s="10"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="16"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="21"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="42"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="41"/>
+      <c r="A17" s="43"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="45"/>
       <c r="E17" s="10"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="14" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H17" s="41"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="44" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H17" s="45"/>
       <c r="I17" s="10"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="21"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="16"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="42"/>
@@ -4777,20 +4802,36 @@
       <c r="K129" s="21"/>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A130" s="43"/>
-      <c r="B130" s="16"/>
-      <c r="C130" s="44"/>
-      <c r="D130" s="45"/>
+      <c r="A130" s="42"/>
+      <c r="B130" s="21"/>
+      <c r="C130" s="14"/>
+      <c r="D130" s="41"/>
       <c r="E130" s="10"/>
-      <c r="F130" s="16"/>
-      <c r="G130" s="44" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H130" s="45"/>
+      <c r="F130" s="21"/>
+      <c r="G130" s="14" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H130" s="41"/>
       <c r="I130" s="10"/>
-      <c r="J130" s="13"/>
-      <c r="K130" s="16"/>
+      <c r="J130" s="12"/>
+      <c r="K130" s="21"/>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A131" s="43"/>
+      <c r="B131" s="16"/>
+      <c r="C131" s="44"/>
+      <c r="D131" s="45"/>
+      <c r="E131" s="10"/>
+      <c r="F131" s="16"/>
+      <c r="G131" s="44" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H131" s="45"/>
+      <c r="I131" s="10"/>
+      <c r="J131" s="13"/>
+      <c r="K131" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>